<commit_message>
Final Revisions to artifacts, inclusion of mp4 from team preso
This commit includes the final revisions to some artifacts, inclusion
of the test cases and traceability artifacts, and the inclusion of
recording from the term project presentation.
</commit_message>
<xml_diff>
--- a/ProjectArtifacts/Group2_Team1_CIList.xlsx
+++ b/ProjectArtifacts/Group2_Team1_CIList.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="-140" windowWidth="14400" windowHeight="14820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="40" yWindow="-140" windowWidth="14400" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CIList" sheetId="1" r:id="rId1"/>
     <sheet name="Version" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130407"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -20,11 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
-  <si>
-    <t>BU Blackboard Team Discussion Board</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t>.XLSX</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,18 +34,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BU Blackboard Team Discussion Board</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Balsamiq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pivotal Tracker - Group 2 team 1 board</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -198,11 +182,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Jeremy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use Case Traceability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jeremy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.XLSX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>github</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>github</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Requirements Traceability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>github</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>revisions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Final</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jeremy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -210,13 +226,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="m/d"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="m/d"/>
+    <numFmt numFmtId="166" formatCode="m/d/yy"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -250,9 +267,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,9 +599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -598,25 +617,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -624,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -633,13 +652,13 @@
         <v>40691</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -647,7 +666,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -656,13 +675,13 @@
         <v>40688</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -670,7 +689,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -679,13 +698,13 @@
         <v>40688</v>
       </c>
       <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
       <c r="G4" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -693,7 +712,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -702,13 +721,13 @@
         <v>40688</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -716,7 +735,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -725,13 +744,13 @@
         <v>40692</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -739,7 +758,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -748,13 +767,13 @@
         <v>41060</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -762,7 +781,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -771,13 +790,13 @@
         <v>40694</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -785,7 +804,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -794,13 +813,13 @@
         <v>40694</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -808,7 +827,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -817,13 +836,13 @@
         <v>40713</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -831,7 +850,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -840,13 +859,13 @@
         <v>40713</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -854,7 +873,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -863,13 +882,13 @@
         <v>40713</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -877,7 +896,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -886,13 +905,13 @@
         <v>40713</v>
       </c>
       <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
       <c r="G13" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -900,7 +919,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -909,13 +928,13 @@
         <v>40713</v>
       </c>
       <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
         <v>34</v>
       </c>
-      <c r="F14" t="s">
-        <v>38</v>
-      </c>
       <c r="G14" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -923,7 +942,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -932,13 +951,13 @@
         <v>40713</v>
       </c>
       <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" t="s">
-        <v>38</v>
-      </c>
       <c r="G15" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -946,7 +965,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -955,17 +974,62 @@
         <v>40713</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>0</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>40715</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>40715</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -978,24 +1042,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1006,28 +1072,41 @@
         <v>40692</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="B3" s="2">
         <v>40713</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>40715</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>